<commit_message>
The sanitization was overkill. restoring files.
</commit_message>
<xml_diff>
--- a/sample_data/sample.xlsx
+++ b/sample_data/sample.xlsx
@@ -25,31 +25,31 @@
     <t>City</t>
   </si>
   <si>
-    <t>John</t>
-  </si>
-  <si>
-    <t>25</t>
-  </si>
-  <si>
-    <t>New York</t>
-  </si>
-  <si>
-    <t>Jane</t>
-  </si>
-  <si>
-    <t>30</t>
-  </si>
-  <si>
-    <t>London</t>
+    <t>Alice</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>Boston</t>
   </si>
   <si>
     <t>Bob</t>
   </si>
   <si>
-    <t>35</t>
-  </si>
-  <si>
-    <t>Paris</t>
+    <t>32</t>
+  </si>
+  <si>
+    <t>Seattle</t>
+  </si>
+  <si>
+    <t>Charlie</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>Austin</t>
   </si>
 </sst>
 </file>

</xml_diff>